<commit_message>
removed bug from parallel sampler. simplified addition of objectives
</commit_message>
<xml_diff>
--- a/cost_db_AMR.xlsx
+++ b/cost_db_AMR.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julie/Documents/coopt/cooptimizer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="0" windowWidth="25600" windowHeight="18480" tabRatio="500"/>
+    <workbookView xWindow="10980" yWindow="1400" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -232,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +251,22 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -268,19 +292,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -609,17 +642,17 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="40.1640625" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +672,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -654,10 +687,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -690,10 +723,10 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -708,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -726,10 +759,10 @@
         <v>4</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -744,10 +777,10 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -762,10 +795,10 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -780,10 +813,10 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -798,10 +831,10 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -816,10 +849,10 @@
         <v>4</v>
       </c>
       <c r="F11" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -834,10 +867,10 @@
         <v>4</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -852,10 +885,10 @@
         <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -870,10 +903,10 @@
         <v>4</v>
       </c>
       <c r="F14" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -888,10 +921,10 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -906,10 +939,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -924,10 +957,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -942,10 +975,10 @@
         <v>4</v>
       </c>
       <c r="F18" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -960,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="F19" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -978,10 +1011,10 @@
         <v>4</v>
       </c>
       <c r="F20" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>61</v>
       </c>
@@ -992,10 +1025,10 @@
         <v>2.85</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>63</v>
       </c>
@@ -1006,10 +1039,10 @@
         <v>2.15</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>65</v>
       </c>
@@ -1025,10 +1058,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>